<commit_message>
Updating stats and datavis
</commit_message>
<xml_diff>
--- a/data/baseInterlabData.xlsx
+++ b/data/baseInterlabData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://saluki-my.sharepoint.com/personal/stantis_siu_edu/Documents/Documents/GitHub/InterLabCompare/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\GitHub\InterLabCompare\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{E75EABCD-9650-43F0-8138-6DA566379326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A81500E7-EB8E-470C-BA20-5755DC3E8E65}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA0FFC8-55FC-4FF8-AB8A-17B8C8CA8B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7020" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="untreated, baked, own rxn" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -372,8 +373,8 @@
   </sheetPr>
   <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2615,4 +2616,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F082F683-43A0-41DB-9EEB-B5E98E005326}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>